<commit_message>
Modify data entry sheets
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/example_sheets.xlsx
+++ b/inst/extdata/Data_entry/example_sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DCC754-1C6D-4DEA-9B7F-83BF4B772914}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA64495-7CD4-4602-B374-CFB8EC69E241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="19080" windowHeight="6820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="19080" windowHeight="6820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_data" sheetId="1" r:id="rId1"/>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1137,7 +1137,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="7">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>6</v>
@@ -1285,7 +1285,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="30">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>75</v>
@@ -1403,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289A40E2-2E80-40B7-B15A-A7ACC55EFECA}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1506,8 +1506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE5508C-700E-4B9F-9966-495F6EFAF069}">
   <dimension ref="A1:BA137"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1518,8 +1518,12 @@
     <col min="4" max="4" width="24.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="8" max="12" width="15.6328125" customWidth="1"/>
+    <col min="7" max="7" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.08984375" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" customWidth="1"/>
+    <col min="11" max="11" width="15.6328125" customWidth="1"/>
+    <col min="12" max="12" width="16.90625" customWidth="1"/>
     <col min="13" max="53" width="10.90625" style="42"/>
   </cols>
   <sheetData>
@@ -2968,7 +2972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>